<commit_message>
Updated EV3 Power Consumption XL Sheet
</commit_message>
<xml_diff>
--- a/EV3_Power_Consumption.xlsx
+++ b/EV3_Power_Consumption.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>9V</t>
   </si>
   <si>
-    <t>8V</t>
-  </si>
-  <si>
     <t>US Sensor</t>
   </si>
   <si>
@@ -87,10 +84,31 @@
     <t>5V</t>
   </si>
   <si>
-    <t>Dexter Industries, Inc.</t>
-  </si>
-  <si>
-    <t>www.dexterindustries.com/ev3.html</t>
+    <t xml:space="preserve">Data by Dexter Industries, 12/2/2013      </t>
+  </si>
+  <si>
+    <t>http://www.dexterindustries.com/ev3.html</t>
+  </si>
+  <si>
+    <t>*1.100</t>
+  </si>
+  <si>
+    <t>*2.620</t>
+  </si>
+  <si>
+    <t>*2.521</t>
+  </si>
+  <si>
+    <t>*1.825</t>
+  </si>
+  <si>
+    <t>7.5V</t>
+  </si>
+  <si>
+    <t>*Exhibited a varying amount of power draw in the motors and "twitching".</t>
+  </si>
+  <si>
+    <t>*2.451</t>
   </si>
 </sst>
 </file>
@@ -429,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -484,11 +502,35 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -552,6 +594,61 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>82919</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>136458</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="ev3 sensors for Dexter Industries"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="619126" y="82919"/>
+          <a:ext cx="695324" cy="644089"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -592,105 +689,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2400300" cy="1419115"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7543800" y="561975"/>
-          <a:ext cx="2400300" cy="1419115"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>495301</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2668852" cy="1590675"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7477126" y="2171700"/>
-          <a:ext cx="2668852" cy="1590675"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>76201</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2714625" cy="1640086"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7334250" y="4248151"/>
-          <a:ext cx="2714625" cy="1640086"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
       <xdr:row>29</xdr:row>
@@ -705,7 +703,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -738,7 +736,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -755,31 +753,36 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3571000" cy="1695618"/>
+      <xdr:colOff>580605</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>8970</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPr id="9" name="Picture 8"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10467975" y="323850"/>
-          <a:ext cx="3571000" cy="1695618"/>
+          <a:off x="152400" y="381000"/>
+          <a:ext cx="3476205" cy="2294970"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -787,7 +790,83 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3905250" y="0"/>
+          <a:ext cx="3000375" cy="1533525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>165598</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638301" y="3495675"/>
+          <a:ext cx="2876550" cy="1241923"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1080,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,24 +1172,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1121,14 +1203,14 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -1146,7 +1228,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="6">
@@ -1167,7 +1249,7 @@
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="11">
@@ -1199,41 +1281,41 @@
     <row r="8" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="20"/>
-      <c r="D8" s="21">
-        <v>0.192</v>
-      </c>
-      <c r="E8" s="21">
-        <v>0.185</v>
-      </c>
-      <c r="F8" s="21">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="22">
-        <v>0.24</v>
+      <c r="D8" s="34">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E8" s="35">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F8" s="35">
+        <v>0.186</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="45">
+        <v>0.24299999999999999</v>
       </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="20"/>
-      <c r="D9" s="23">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="E9" s="23">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="F9" s="23">
-        <v>0.17</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="24">
+      <c r="D9" s="37">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="E9" s="38">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F9" s="38">
+        <v>0.18</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="47">
         <v>0.23599999999999999</v>
       </c>
       <c r="I9" s="1"/>
@@ -1241,42 +1323,42 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="23">
-        <v>0.28199999999999997</v>
-      </c>
-      <c r="E10" s="23">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="F10" s="23">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="24">
-        <v>0.32</v>
+      <c r="D10" s="37">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E10" s="38">
+        <v>0.31</v>
+      </c>
+      <c r="F10" s="38">
+        <v>0.27</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="47">
+        <v>0.34100000000000003</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="10"/>
-      <c r="D11" s="11">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="E11" s="11">
-        <v>0.21</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0.21099999999999999</v>
-      </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="25">
-        <v>0.26</v>
+      <c r="D11" s="39">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="40">
+        <v>0.249</v>
+      </c>
+      <c r="F11" s="40">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="G11" s="41"/>
+      <c r="H11" s="49">
+        <v>0.27500000000000002</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -1284,94 +1366,94 @@
       <c r="A12" s="1"/>
       <c r="B12" s="14"/>
       <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="44"/>
       <c r="H12" s="18"/>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="20"/>
-      <c r="D13" s="21">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="21">
-        <v>0.91</v>
-      </c>
-      <c r="F13" s="21">
-        <v>0.93</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="22">
-        <v>0.99</v>
+      <c r="D13" s="35">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="E13" s="35">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="F13" s="35">
+        <v>0.98</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="45">
+        <v>0.995</v>
       </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="20"/>
-      <c r="D14" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="E14" s="23">
-        <v>1.6</v>
-      </c>
-      <c r="F14" s="23">
-        <v>1.653</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="24">
-        <v>0.99</v>
+      <c r="D14" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="36"/>
+      <c r="H14" s="46">
+        <v>1.75</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="20"/>
-      <c r="D15" s="23">
-        <v>0.9</v>
-      </c>
-      <c r="E15" s="23">
-        <v>0.75</v>
-      </c>
-      <c r="F15" s="23">
-        <v>0.71</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="24">
-        <v>0.7</v>
+      <c r="D15" s="38">
+        <v>0.84</v>
+      </c>
+      <c r="E15" s="38">
+        <v>0.78</v>
+      </c>
+      <c r="F15" s="38">
+        <v>0.745</v>
+      </c>
+      <c r="G15" s="36"/>
+      <c r="H15" s="47">
+        <v>0.60099999999999998</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="11">
-        <v>2.35</v>
-      </c>
-      <c r="E16" s="11">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="F16" s="11">
-        <v>2.3650000000000002</v>
-      </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13">
-        <v>2</v>
+      <c r="D16" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="41"/>
+      <c r="H16" s="48">
+        <v>2.1800000000000002</v>
       </c>
       <c r="I16" s="1"/>
     </row>
@@ -1389,11 +1471,11 @@
     <row r="18" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="19" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="21">
-        <v>0.99</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="E18" s="21">
         <v>0.11</v>
@@ -1410,11 +1492,11 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="23">
-        <v>0.96</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="E19" s="23">
         <v>0.104</v>
@@ -1431,11 +1513,11 @@
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="11">
-        <v>0.87</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="E20" s="11">
         <v>9.9000000000000005E-2</v>
@@ -1463,14 +1545,14 @@
     <row r="22" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="21">
-        <v>0.86</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="E22" s="21">
-        <v>0.95</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="F22" s="21">
         <v>9.8000000000000004E-2</v>
@@ -1484,7 +1566,7 @@
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="29">
@@ -1515,38 +1597,73 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="D25" s="32" t="s">
+        <v>23</v>
+      </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="34">
-        <v>41610</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="s">
-        <v>24</v>
-      </c>
+      <c r="A29" s="1"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:H2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B29" r:id="rId1"/>
+    <hyperlink ref="D25" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
@@ -1566,12 +1683,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1583,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:O54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>